<commit_message>
fix(back): #2211.5 extra xls report checks
- Template modified: wider Where column &
shorter Treatment manager one


Former-commit-id: c72cc9e9bce3217a1815263667cff421abab5a8f
</commit_message>
<xml_diff>
--- a/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
+++ b/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
@@ -562,27 +562,27 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.11320754716981"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.1933962264151"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.0141509433962"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="26.8349056603774"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="69.2641509433962"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="37.938679245283"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.6981132075472"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="43.8066037735849"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="35.75"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.188679245283"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="35.3207547169811"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="77.377358490566"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="35.3207547169811"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="76.2547169811321"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.35849056603774"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.48584905660377"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.5188679245283"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.1320754716981"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="28.0801886792453"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="72.3867924528302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="39.688679245283"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="33.0707547169811"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="45.6792452830189"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="37.3160377358491"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="25.3349056603774"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="36.9433962264151"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="80.872641509434"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="36.9433962264151"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="61.0141509433962"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.73584905660377"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -659,8 +659,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.7735849056604"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.35849056603774"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6415094339623"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.73584905660377"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refac(back): #2211.7 change sheet name
- CVSS label also


Former-commit-id: 5362ff52de558a041ba5063927608ea032ac3935
</commit_message>
<xml_diff>
--- a/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
+++ b/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Findings" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="CVSSv3" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">Severity</t>
   </si>
   <si>
-    <t xml:space="preserve">CVSSv3 Vector</t>
+    <t xml:space="preserve">CVSSv3.1 Vector</t>
   </si>
   <si>
     <t xml:space="preserve">Pending Reattack</t>
@@ -563,26 +563,26 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.48584905660377"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.5188679245283"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.1320754716981"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="28.0801886792453"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="72.3867924528302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="39.688679245283"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="33.0707547169811"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="45.6792452830189"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="37.3160377358491"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="25.3349056603774"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="36.9433962264151"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="80.872641509434"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="36.9433962264151"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="61.0141509433962"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.73584905660377"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.23584905660377"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.6509433962264"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.872641509434"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="30.7028301886792"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="79"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="43.1839622641509"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.1933962264151"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="49.6698113207547"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="40.6839622641509"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.5801886792453"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="40.311320754717"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="88.2358490566038"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="40.311320754717"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="66.3962264150943"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.4858490566038"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -659,8 +659,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6415094339623"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.73584905660377"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.7594339622642"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.4858490566038"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat(back): #2268 new xls set of columns
- A variety of new columns added to report
- Write row function splitted by column groups
- Add cell function modified to include an align
attribute distinguishing between centered fields
and left-align ones
- Header color changed to the red one used
in Integrates


Former-commit-id: da0f2a5c0cb04d53efe180d3006d4859bcb6569c
</commit_message>
<xml_diff>
--- a/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
+++ b/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
@@ -21,15 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="88">
   <si>
     <t xml:space="preserve">#</t>
   </si>
   <si>
+    <t xml:space="preserve">Related Finding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding Id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Where</t>
   </si>
   <si>
-    <t xml:space="preserve">Related Finding</t>
+    <t xml:space="preserve">Vulnerability Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -38,37 +47,100 @@
     <t xml:space="preserve">Severity</t>
   </si>
   <si>
-    <t xml:space="preserve">CVSSv3.1 Vector</t>
+    <t xml:space="preserve">Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affected System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External BTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compromised Attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Compromised records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close Moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age in days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Treatment Moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Treatment Justification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Treatment expiration Moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Treatment manager</t>
   </si>
   <si>
     <t xml:space="preserve">Pending Reattack</t>
   </si>
   <si>
-    <t xml:space="preserve">Is Exploitable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age (days)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment justification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment expiration date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment manager</t>
+    <t xml:space="preserve"># Requested Reattacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last requested reattack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last reattack Requester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVSSv3.1 string vector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack Vector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack Complexity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privileges Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severity Scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confidentiality Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrity Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploitability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remediation Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Confidence</t>
   </si>
   <si>
     <t xml:space="preserve">Reference sheet for criticality calculation</t>
@@ -83,9 +155,6 @@
     <t xml:space="preserve">Option</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack Vector</t>
-  </si>
-  <si>
     <t xml:space="preserve">AV</t>
   </si>
   <si>
@@ -101,9 +170,6 @@
     <t xml:space="preserve">Physical</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack Complexity</t>
-  </si>
-  <si>
     <t xml:space="preserve">AC</t>
   </si>
   <si>
@@ -122,9 +188,6 @@
     <t xml:space="preserve">None</t>
   </si>
   <si>
-    <t xml:space="preserve">User Interaction</t>
-  </si>
-  <si>
     <t xml:space="preserve">UI</t>
   </si>
   <si>
@@ -143,21 +206,12 @@
     <t xml:space="preserve">Changed</t>
   </si>
   <si>
-    <t xml:space="preserve">Confidentiality Impact</t>
-  </si>
-  <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">Integrity Impact</t>
-  </si>
-  <si>
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">Availability Impact</t>
-  </si>
-  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
@@ -176,9 +230,6 @@
     <t xml:space="preserve">Unproven</t>
   </si>
   <si>
-    <t xml:space="preserve">Remediation Level</t>
-  </si>
-  <si>
     <t xml:space="preserve">RL</t>
   </si>
   <si>
@@ -192,9 +243,6 @@
   </si>
   <si>
     <t xml:space="preserve">Oficial Fix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Confidence</t>
   </si>
   <si>
     <t xml:space="preserve">RC</t>
@@ -269,14 +317,8 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -284,6 +326,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -291,14 +334,19 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="14"/>
+      <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -347,12 +395,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAFABAB"/>
-        <bgColor rgb="FF969696"/>
+        <fgColor rgb="FFFF3435"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -365,6 +413,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -423,11 +478,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,15 +494,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -451,35 +506,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,7 +563,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFAFABAB"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -539,7 +594,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3435"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -560,29 +615,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J:J"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="50.4"/>
+  <sheetFormatPr defaultRowHeight="93.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.23584905660377"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.6509433962264"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.872641509434"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="30.7028301886792"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="79"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="43.1839622641509"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.1933962264151"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="49.6698113207547"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.7311320754717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="78.127358490566"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.7028301886792"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="97.0990566037736"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="75.3820754716981"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="111.448113207547"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.2075471698113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.3396226415094"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="180.641509433962"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="40.6839622641509"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.5801886792453"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="40.311320754717"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="88.2358490566038"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="40.311320754717"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="66.3962264150943"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.4858490566038"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="39.688679245283"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="61.4056603773585"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="83.9905660377358"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="96.872641509434"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="55.4150943396226"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.8490566037736"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="40.438679245283"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="42.0188679245283"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="16.8584905660377"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="20.7169811320755"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="42.9339622641509"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="125.551886792453"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="56.4103773584906"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="67.1462264150943"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.5943396226415"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="19.4716981132075"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="35.8207547169811"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="81.122641509434"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="84.6179245283019"/>
+    <col collapsed="false" hidden="false" max="34" min="30" style="1" width="14.6037735849057"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="17.7216981132075"/>
+    <col collapsed="false" hidden="false" max="37" min="36" style="1" width="14.6037735849057"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="16.4764150943396"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="1" width="14.6037735849057"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="2" width="11.3584905660377"/>
+    <col collapsed="false" hidden="false" max="1025" min="42" style="0" width="8.98584905660377"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -604,7 +680,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -633,6 +709,78 @@
       </c>
       <c r="P1" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -653,19 +801,19 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="J:J A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.7594339622642"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.4858490566038"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.584905660377"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.98584905660377"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -683,13 +831,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -697,199 +845,199 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -903,13 +1051,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -917,10 +1065,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>0.85</v>
@@ -937,10 +1085,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>0.77</v>
@@ -953,10 +1101,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C19" s="15" t="n">
         <v>0.85</v>
@@ -971,10 +1119,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>0.85</v>
@@ -987,10 +1135,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C21" s="15" t="n">
         <v>0</v>
@@ -1003,10 +1151,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C22" s="15" t="n">
         <v>0.56</v>
@@ -1021,10 +1169,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>0.56</v>
@@ -1039,10 +1187,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C24" s="15" t="n">
         <v>0.56</v>
@@ -1057,10 +1205,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C25" s="15" t="n">
         <v>1</v>
@@ -1077,10 +1225,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>1</v>
@@ -1097,10 +1245,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>1</v>
@@ -1123,13 +1271,13 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1137,199 +1285,199 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="F40" s="10"/>
     </row>

</xml_diff>

<commit_message>
integrates\feat(back): #2268.4 new columns for xls report
- Tags, business critically, remediation ratio
- Where and specific splitted in two columns


Former-commit-id: e43389429ff56ad0bb4c1d60e3f6bd8abdf51b19
</commit_message>
<xml_diff>
--- a/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
+++ b/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="92">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -32,10 +32,13 @@
     <t xml:space="preserve">Finding Id</t>
   </si>
   <si>
+    <t xml:space="preserve">Vulnerability Id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Where</t>
   </si>
   <si>
-    <t xml:space="preserve">Vulnerability Id</t>
+    <t xml:space="preserve">Specific</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -71,6 +74,12 @@
     <t xml:space="preserve"># Compromised records</t>
   </si>
   <si>
+    <t xml:space="preserve">Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Critically</t>
+  </si>
+  <si>
     <t xml:space="preserve">Report Moment</t>
   </si>
   <si>
@@ -99,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve"># Requested Reattacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remediation Effectiveness</t>
   </si>
   <si>
     <t xml:space="preserve">Last requested reattack</t>
@@ -615,50 +627,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J:J"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="93.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.7311320754717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="78.127358490566"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.7028301886792"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="97.0990566037736"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="75.3820754716981"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="111.448113207547"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.2075471698113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.3396226415094"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="180.641509433962"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="40.6839622641509"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="39.688679245283"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="61.4056603773585"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="83.9905660377358"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="96.872641509434"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="55.4150943396226"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.8490566037736"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="40.438679245283"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="42.0188679245283"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="16.8584905660377"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="20.7169811320755"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="42.9339622641509"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="125.551886792453"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="56.4103773584906"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="67.1462264150943"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.5943396226415"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="19.4716981132075"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="35.8207547169811"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="81.122641509434"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="84.6179245283019"/>
-    <col collapsed="false" hidden="false" max="34" min="30" style="1" width="14.6037735849057"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="17.7216981132075"/>
-    <col collapsed="false" hidden="false" max="37" min="36" style="1" width="14.6037735849057"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="16.4764150943396"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="1" width="14.6037735849057"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="2" width="11.3584905660377"/>
-    <col collapsed="false" hidden="false" max="1025" min="42" style="0" width="8.98584905660377"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4716981132075"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="116.066037735849"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.4339622641509"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="92.5943396226415"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="93.127358490566"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="74.933962264151"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="165.11320754717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.938679245283"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.0707547169811"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="230.264150943396"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="59.4056603773585"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="58.0330188679245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="90.8584905660377"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="124.801886792453"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="143.77358490566"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="81.4952830188679"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.7122641509434"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="77.627358490566"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="27.0801886792453"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="59.2830188679245"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="61.5283018867925"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="24.7122641509434"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="30.7028301886792"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="62.7783018867925"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="186.457547169811"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="83.4952830188679"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="99.4669811320755"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="27.4575471698113"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="28.7028301886792"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="21.9669811320755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="52.6650943396226"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="120.433962264151"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="125.679245283019"/>
+    <col collapsed="false" hidden="false" max="38" min="34" style="1" width="21.3396226415094"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="25.9575471698113"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="1" width="21.3396226415094"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="24.3349056603774"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="1" width="21.3396226415094"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="2" width="16.4764150943396"/>
+    <col collapsed="false" hidden="false" max="1025" min="46" style="0" width="10.1084905660377"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -677,7 +693,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -713,7 +729,7 @@
       <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -781,6 +797,18 @@
       </c>
       <c r="AN1" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -802,18 +830,18 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="J:J A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.584905660377"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.98584905660377"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="155.132075471698"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1084905660377"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -831,13 +859,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -845,199 +873,199 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -1051,13 +1079,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1065,10 +1093,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>0.85</v>
@@ -1085,10 +1113,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>0.77</v>
@@ -1101,10 +1129,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C19" s="15" t="n">
         <v>0.85</v>
@@ -1119,10 +1147,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>0.85</v>
@@ -1135,10 +1163,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C21" s="15" t="n">
         <v>0</v>
@@ -1151,10 +1179,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C22" s="15" t="n">
         <v>0.56</v>
@@ -1169,10 +1197,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>0.56</v>
@@ -1187,10 +1215,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C24" s="15" t="n">
         <v>0.56</v>
@@ -1205,10 +1233,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C25" s="15" t="n">
         <v>1</v>
@@ -1225,10 +1253,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>1</v>
@@ -1245,10 +1273,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>1</v>
@@ -1271,13 +1299,13 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1285,199 +1313,199 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D38" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="F38" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F40" s="10"/>
     </row>

</xml_diff>

<commit_message>
integrates\refac(back): #2268.6 reduce code length
- Row fields grouped and looped through
- Template slightly modified


Former-commit-id: f2cddc79f559d3f0a093acc89da97e7b05beb730
</commit_message>
<xml_diff>
--- a/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
+++ b/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
@@ -633,57 +633,56 @@
   </sheetPr>
   <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="27" zoomScaleNormal="27" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="1" sqref="2:1048576 V1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="93.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.2216981132075"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="121.311320754717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.1792452830189"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="96.7216981132076"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="97.3490566037736"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="78.25"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="172.603773584906"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="40.6839622641509"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="34.5707547169811"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="240.622641509434"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="62.0283018867925"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="60.5283018867925"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="94.9764150943396"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="130.297169811321"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="150.264150943396"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="85.1179245283019"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="25.8349056603774"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="81.122641509434"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="28.3301886792453"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="61.9009433962264"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="64.2735849056604"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="25.8349056603774"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="32.0754716981132"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="69.4575471698113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="216.47641509434"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="85.1556603773585"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="115.608490566038"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="32.0754716981132"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="65.5235849056604"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="194.943396226415"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="87.2358490566038"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="103.962264150943"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="28.7028301886792"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="29.9528301886792"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="22.9622641509434"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="54.9150943396226"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="125.801886792453"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="131.292452830189"/>
-    <col collapsed="false" hidden="false" max="43" min="39" style="1" width="22.3396226415094"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="27.0801886792453"/>
-    <col collapsed="false" hidden="false" max="46" min="45" style="1" width="22.3396226415094"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="25.4622641509434"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="1" width="22.3396226415094"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="2" width="17.2216981132075"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="10.4858490566038"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.0943396226415"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="126.674528301887"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="46.0518867924528"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="101.089622641509"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="101.716981132075"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="81.7452830188679"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="180.339622641509"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.4669811320755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.1933962264151"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="225.485849056604"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="64.7735849056604"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="63.1509433962264"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="99.2169811320755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="136.037735849057"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="157.004716981132"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="88.9858490566038"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="26.9575471698113"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="84.7405660377359"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="29.5801886792453"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="64.6462264150943"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="67.1462264150943"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="26.9575471698113"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="33.5707547169811"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="72.6367924528302"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="226.268867924528"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="88.9858490566038"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="120.811320754717"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="33.5707547169811"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="68.3915094339623"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="203.801886792453"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="91.1084905660377"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="87.622641509434"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="26.1509433962264"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="25.9198113207547"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="26.1509433962264"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="57.2830188679245"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="100.466981132075"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="112.853773584906"/>
+    <col collapsed="false" hidden="false" max="43" min="39" style="1" width="23.3396226415094"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="28.3301886792453"/>
+    <col collapsed="false" hidden="false" max="46" min="45" style="1" width="23.3396226415094"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="24.5424528301887"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="1" width="23.3396226415094"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="2" width="17.9716981132075"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -853,14 +852,13 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="27" zoomScaleNormal="27" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="2:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="162.117924528302"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.4858490566038"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="169.358490566038"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
integrates\feat(back): #2268.7 new xls generation method
- openpyxls developers recommend to use WriteOnlyWorksheet in
that cases where large xls files are handled for writting
purposes, because of it's performance
- Achieving this means that we need a single file for reading and
another one for writing, not only one for both
things. Thath's why I've created a workbook to work with instead
of rawly use the template
- Implementing this causes that we dont generate this report
by cells, so by rows
- All the style of the cells and rows is now made directly
in the code, so maybe we can easily change that stuff
- It's supossed that by using this we generate xls reports
fastly
- Next work will be on refactoring and cleaning code
- pylint exceptions for some openpyxls style properties


Former-commit-id: c39dd6c99c4c24aabd1518cf1bc3f60e90ccf3db
</commit_message>
<xml_diff>
--- a/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
+++ b/django-apps/integrates-back-async/backend/reports/templates/excel/TECHNICAL_VULNS.xlsx
@@ -633,56 +633,63 @@
   </sheetPr>
   <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH1" activeCellId="0" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="93.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.0943396226415"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="126.674528301887"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="46.0518867924528"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="101.089622641509"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="101.716981132075"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="81.7452830188679"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="180.339622641509"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.4669811320755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.1933962264151"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="225.485849056604"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="64.7735849056604"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="63.1509433962264"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="99.2169811320755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="136.037735849057"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="157.004716981132"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="88.9858490566038"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="26.9575471698113"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="84.7405660377359"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="29.5801886792453"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="64.6462264150943"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="67.1462264150943"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="26.9575471698113"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="33.5707547169811"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="72.6367924528302"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="226.268867924528"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="88.9858490566038"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="120.811320754717"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="33.5707547169811"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="68.3915094339623"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="203.801886792453"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="91.1084905660377"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="87.622641509434"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="26.1509433962264"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="25.9198113207547"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="26.1509433962264"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="57.2830188679245"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="100.466981132075"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="112.853773584906"/>
-    <col collapsed="false" hidden="false" max="43" min="39" style="1" width="23.3396226415094"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="28.3301886792453"/>
-    <col collapsed="false" hidden="false" max="46" min="45" style="1" width="23.3396226415094"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="24.5424528301887"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="1" width="23.3396226415094"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="2" width="17.9716981132075"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8396226415094"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="138.155660377359"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.1698113207547"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="110.452830188679"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="111.075471698113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="89.2358490566038"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="196.938679245283"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="39.811320754717"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.561320754717"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="246.235849056604"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="70.6367924528302"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="68.7688679245283"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="108.452830188679"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="148.514150943396"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="171.481132075472"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="97.0990566037736"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="58.7830188679245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="92.4811320754717"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="58.7830188679245"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="70.5141509433962"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="73.2594339622642"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="43.1839622641509"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="57.4103773584906"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="79.25"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="247.11320754717"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="97.0990566037736"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="131.792452830189"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="75.3820754716981"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="74.5094339622642"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="222.52358490566"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="99.4669811320755"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="95.5990566037736"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="80.2830188679245"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="81.4905660377358"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="74.5094339622642"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="62.4009433962264"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="109.702830188679"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="123.306603773585"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="74.5094339622642"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="96.3396226415094"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="87.9103773584906"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="78.6745283018868"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="80.2830188679245"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="84.3018867924528"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="1" width="81.8867924528302"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="74.5094339622642"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="82.2877358490566"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="1" width="83.8915094339623"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="1" width="84.6981132075472"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="2" width="19.5943396226415"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.35849056603774"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -852,13 +859,14 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="169.358490566038"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="184.957547169811"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.35849056603774"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>